<commit_message>
Added Median Tax and Median Monthly Housing Cost data
Added Median Tax and Median Monthly Housing Cost aggregate data from the US Census ACS survey for the top 70+ most populous cities in the USA.
</commit_message>
<xml_diff>
--- a/Datasets/FINAL_Median_Income_ACS_Supplemented_by_SAIPE.xlsx
+++ b/Datasets/FINAL_Median_Income_ACS_Supplemented_by_SAIPE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ea8e7c1a7f050da2/Documents/GitHub/project-one/Datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="8_{D2CAA6D8-C77E-4D44-9783-11BC20EDE6C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9B588E39-A84A-4813-9A64-05835248BA45}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="8_{D2CAA6D8-C77E-4D44-9783-11BC20EDE6C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4238693C-74CB-482C-8D15-5F2A9E982470}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7581,8 +7581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J782"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E71" sqref="E71:E544"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Sorted and Corrected Median Tax Data
Sorted the lists and corrected 2020 and 2021 median tax data
</commit_message>
<xml_diff>
--- a/Datasets/FINAL_Median_Income_ACS_Supplemented_by_SAIPE.xlsx
+++ b/Datasets/FINAL_Median_Income_ACS_Supplemented_by_SAIPE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ea8e7c1a7f050da2/Documents/GitHub/project-one/Datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="8_{D2CAA6D8-C77E-4D44-9783-11BC20EDE6C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DD20864A-FB96-47BD-8FF2-5480BE6F28DD}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="8_{D2CAA6D8-C77E-4D44-9783-11BC20EDE6C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7C2410CE-0C3E-41EF-B702-839D805DDCF1}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7592,7 +7592,7 @@
   <dimension ref="A1:J782"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>